<commit_message>
Lots of new functionality - way too long between commits
</commit_message>
<xml_diff>
--- a/burner/docs/zoomcalcs.xlsx
+++ b/burner/docs/zoomcalcs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="51540" yWindow="0" windowWidth="42080" windowHeight="26820" tabRatio="500"/>
+    <workbookView xWindow="54600" yWindow="640" windowWidth="42080" windowHeight="26820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Zoom Calcs" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>0,0</t>
   </si>
@@ -131,12 +131,15 @@
   <si>
     <t>ImageMagick</t>
   </si>
+  <si>
+    <t xml:space="preserve">Invalidation Areas </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -204,6 +207,12 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -233,7 +242,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -388,8 +397,502 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -401,8 +904,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -430,17 +939,168 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="29" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="30" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="32" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="33" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="34" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="35" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="36" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="37" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="38" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="39" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="40" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="41" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="42" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="43" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="44" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="45" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="46" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="47" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="48" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="49" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="50" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="51" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="17">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
     <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2100,13 +2760,13 @@
     </dgm:pt>
   </dgm:ptLst>
   <dgm:cxnLst>
-    <dgm:cxn modelId="{FBC10F71-79CE-BF4F-88E1-8B338B96B46B}" srcId="{04AC73EE-BDC1-384B-8549-50C34A039332}" destId="{8CEDD984-2F92-F04E-A5F1-EDA24992D79B}" srcOrd="0" destOrd="0" parTransId="{3E2FB207-8794-FB4C-83E7-E292E1527B17}" sibTransId="{8D13B74C-F147-5E48-A9EE-99A8DEF81680}"/>
     <dgm:cxn modelId="{DC49B343-FFD4-C344-8DE0-9E7C12EF24F3}" type="presOf" srcId="{8CEDD984-2F92-F04E-A5F1-EDA24992D79B}" destId="{807F8D39-CEB8-D94E-ADA0-B5DAB91CE6D4}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/pyramid1"/>
-    <dgm:cxn modelId="{C76569C1-3390-FC4B-B69A-66DA483086C6}" type="presOf" srcId="{56FF6EDA-C426-1947-B0BC-F1FD5537EBDA}" destId="{9232989E-0F4A-AB4A-8BAB-169A02E5342D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/pyramid1"/>
-    <dgm:cxn modelId="{66A42066-B451-454A-9279-174191947194}" srcId="{04AC73EE-BDC1-384B-8549-50C34A039332}" destId="{56FF6EDA-C426-1947-B0BC-F1FD5537EBDA}" srcOrd="1" destOrd="0" parTransId="{5000B324-3AC6-1F41-8AB5-AABFB7D0ED29}" sibTransId="{C1E293B3-FF0A-014F-8AA8-96F38A4F635E}"/>
     <dgm:cxn modelId="{66949C84-460B-D943-A58D-EE3123AABE5D}" type="presOf" srcId="{04AC73EE-BDC1-384B-8549-50C34A039332}" destId="{B0F469D0-E918-4548-B12D-78E42CFB4EEC}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/pyramid1"/>
     <dgm:cxn modelId="{677C22A1-2074-5F43-9B90-B81494DDEDCC}" type="presOf" srcId="{56FF6EDA-C426-1947-B0BC-F1FD5537EBDA}" destId="{0A702D6B-CA8B-B244-9C86-E8C458B7DD73}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/pyramid1"/>
+    <dgm:cxn modelId="{66A42066-B451-454A-9279-174191947194}" srcId="{04AC73EE-BDC1-384B-8549-50C34A039332}" destId="{56FF6EDA-C426-1947-B0BC-F1FD5537EBDA}" srcOrd="1" destOrd="0" parTransId="{5000B324-3AC6-1F41-8AB5-AABFB7D0ED29}" sibTransId="{C1E293B3-FF0A-014F-8AA8-96F38A4F635E}"/>
+    <dgm:cxn modelId="{FBC10F71-79CE-BF4F-88E1-8B338B96B46B}" srcId="{04AC73EE-BDC1-384B-8549-50C34A039332}" destId="{8CEDD984-2F92-F04E-A5F1-EDA24992D79B}" srcOrd="0" destOrd="0" parTransId="{3E2FB207-8794-FB4C-83E7-E292E1527B17}" sibTransId="{8D13B74C-F147-5E48-A9EE-99A8DEF81680}"/>
     <dgm:cxn modelId="{7E214855-F841-9947-B6BB-A46919CC396C}" type="presOf" srcId="{8CEDD984-2F92-F04E-A5F1-EDA24992D79B}" destId="{805B12C5-67F2-8D44-BCE2-81C3E276B345}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/pyramid1"/>
+    <dgm:cxn modelId="{C76569C1-3390-FC4B-B69A-66DA483086C6}" type="presOf" srcId="{56FF6EDA-C426-1947-B0BC-F1FD5537EBDA}" destId="{9232989E-0F4A-AB4A-8BAB-169A02E5342D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/pyramid1"/>
     <dgm:cxn modelId="{BFF5AC6C-478C-CB4C-97BB-F09CA583524A}" type="presParOf" srcId="{B0F469D0-E918-4548-B12D-78E42CFB4EEC}" destId="{9EDDC16C-73EC-244E-B38F-FB8AB47B4531}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/pyramid1"/>
     <dgm:cxn modelId="{F48048B7-DE82-8543-9DB0-D880E2BE5858}" type="presParOf" srcId="{9EDDC16C-73EC-244E-B38F-FB8AB47B4531}" destId="{805B12C5-67F2-8D44-BCE2-81C3E276B345}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/pyramid1"/>
     <dgm:cxn modelId="{A4BCA4E4-6E9C-7A4E-AC9C-80C3348B8835}" type="presParOf" srcId="{9EDDC16C-73EC-244E-B38F-FB8AB47B4531}" destId="{807F8D39-CEB8-D94E-ADA0-B5DAB91CE6D4}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/pyramid1"/>
@@ -2225,6 +2885,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{5DF3CB97-E24D-994F-BF96-FECCDB7FC9A8}" type="pres">
       <dgm:prSet presAssocID="{E04DD675-0C89-ED41-9D34-B1DA75C31CCE}" presName="levelTx" presStyleLbl="revTx" presStyleIdx="0" presStyleCnt="0">
@@ -2234,6 +2901,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{9AA9C140-3F9A-8649-8EE8-70453A632372}" type="pres">
       <dgm:prSet presAssocID="{8EE2FE12-BD10-6442-A42B-1EF1715AF6BB}" presName="Name8" presStyleCnt="0"/>
@@ -2247,6 +2921,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{BCE80ADE-2EAB-D146-B1E8-CED790E579DA}" type="pres">
       <dgm:prSet presAssocID="{8EE2FE12-BD10-6442-A42B-1EF1715AF6BB}" presName="levelTx" presStyleLbl="revTx" presStyleIdx="0" presStyleCnt="0">
@@ -2256,16 +2937,23 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
   </dgm:ptLst>
   <dgm:cxnLst>
-    <dgm:cxn modelId="{817B8982-B679-824F-8EEC-D676CD582C6B}" type="presOf" srcId="{8EE2FE12-BD10-6442-A42B-1EF1715AF6BB}" destId="{30E4E314-A92F-904C-B115-6A05ED29629A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/pyramid1"/>
+    <dgm:cxn modelId="{F365A452-D5D2-954A-8FF9-ED26A02DDF61}" type="presOf" srcId="{D473421F-A8D3-4A43-A5CE-656210C4905C}" destId="{F3E58A83-AE87-2743-8A8E-DF058391B41B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/pyramid1"/>
+    <dgm:cxn modelId="{8506E437-73CB-7641-A5EF-B52856B5741B}" type="presOf" srcId="{8EE2FE12-BD10-6442-A42B-1EF1715AF6BB}" destId="{BCE80ADE-2EAB-D146-B1E8-CED790E579DA}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/pyramid1"/>
     <dgm:cxn modelId="{8FA3FC3C-8008-2B45-9B05-65CDC6EA4E3A}" srcId="{D473421F-A8D3-4A43-A5CE-656210C4905C}" destId="{E04DD675-0C89-ED41-9D34-B1DA75C31CCE}" srcOrd="0" destOrd="0" parTransId="{E1945D7B-C2E1-E544-BC61-B206E64CFCAC}" sibTransId="{FF526742-BE9D-FF41-A689-A982EAC0E82F}"/>
     <dgm:cxn modelId="{200E03B5-C40B-EA4F-A61E-D686DB9E0406}" type="presOf" srcId="{E04DD675-0C89-ED41-9D34-B1DA75C31CCE}" destId="{E2A376BB-F5AE-7F4A-838F-B60DE8C91898}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/pyramid1"/>
-    <dgm:cxn modelId="{8506E437-73CB-7641-A5EF-B52856B5741B}" type="presOf" srcId="{8EE2FE12-BD10-6442-A42B-1EF1715AF6BB}" destId="{BCE80ADE-2EAB-D146-B1E8-CED790E579DA}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/pyramid1"/>
+    <dgm:cxn modelId="{9C25B6C4-E2D3-B249-A1FA-CFC601247890}" type="presOf" srcId="{E04DD675-0C89-ED41-9D34-B1DA75C31CCE}" destId="{5DF3CB97-E24D-994F-BF96-FECCDB7FC9A8}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/pyramid1"/>
+    <dgm:cxn modelId="{817B8982-B679-824F-8EEC-D676CD582C6B}" type="presOf" srcId="{8EE2FE12-BD10-6442-A42B-1EF1715AF6BB}" destId="{30E4E314-A92F-904C-B115-6A05ED29629A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/pyramid1"/>
     <dgm:cxn modelId="{72EBB228-0D27-3240-95C6-8CB8C0915E9E}" srcId="{D473421F-A8D3-4A43-A5CE-656210C4905C}" destId="{8EE2FE12-BD10-6442-A42B-1EF1715AF6BB}" srcOrd="1" destOrd="0" parTransId="{3169BE33-D13D-C947-AAE2-88C0FA38B575}" sibTransId="{602C8988-6DD5-D145-94B7-FA95D9A45563}"/>
-    <dgm:cxn modelId="{F365A452-D5D2-954A-8FF9-ED26A02DDF61}" type="presOf" srcId="{D473421F-A8D3-4A43-A5CE-656210C4905C}" destId="{F3E58A83-AE87-2743-8A8E-DF058391B41B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/pyramid1"/>
-    <dgm:cxn modelId="{9C25B6C4-E2D3-B249-A1FA-CFC601247890}" type="presOf" srcId="{E04DD675-0C89-ED41-9D34-B1DA75C31CCE}" destId="{5DF3CB97-E24D-994F-BF96-FECCDB7FC9A8}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/pyramid1"/>
     <dgm:cxn modelId="{05C696C6-C8B8-1E4F-86DD-0E17C232F0AB}" type="presParOf" srcId="{F3E58A83-AE87-2743-8A8E-DF058391B41B}" destId="{E1992E6B-46E3-EC49-A5F7-85E602B7D22F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/pyramid1"/>
     <dgm:cxn modelId="{D0624A07-45DE-1E40-8745-88B3AB851465}" type="presParOf" srcId="{E1992E6B-46E3-EC49-A5F7-85E602B7D22F}" destId="{E2A376BB-F5AE-7F4A-838F-B60DE8C91898}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/pyramid1"/>
     <dgm:cxn modelId="{D1AE2833-7903-FE4D-AD38-B9EABED3A7CE}" type="presParOf" srcId="{E1992E6B-46E3-EC49-A5F7-85E602B7D22F}" destId="{5DF3CB97-E24D-994F-BF96-FECCDB7FC9A8}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/pyramid1"/>
@@ -5622,10 +6310,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:X66"/>
+  <dimension ref="B2:X90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N78" sqref="N78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5947,7 +6635,7 @@
         <v>512</v>
       </c>
       <c r="N32" s="4">
-        <f t="shared" ref="N32:N49" si="1">M32*0.3</f>
+        <f t="shared" ref="N32:N46" si="1">M32*0.3</f>
         <v>153.6</v>
       </c>
       <c r="O32" s="4"/>
@@ -5970,7 +6658,7 @@
         <v>2</v>
       </c>
       <c r="M33" s="4">
-        <f t="shared" ref="M33:M49" si="2">M32*2</f>
+        <f t="shared" ref="M33:M46" si="2">M32*2</f>
         <v>1024</v>
       </c>
       <c r="N33" s="4">
@@ -6316,7 +7004,7 @@
         <v>4</v>
       </c>
       <c r="G49">
-        <f t="shared" ref="G49:G54" si="7">ROUNDUP( LOG( C49/256, 2), 0)</f>
+        <f t="shared" ref="G49:G50" si="7">ROUNDUP( LOG( C49/256, 2), 0)</f>
         <v>4</v>
       </c>
       <c r="O49" s="4"/>
@@ -6533,7 +7221,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="12:17">
+    <row r="65" spans="3:17">
       <c r="L65">
         <v>9000</v>
       </c>
@@ -6549,7 +7237,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="12:17">
+    <row r="66" spans="3:17">
       <c r="L66">
         <v>14000</v>
       </c>
@@ -6563,6 +7251,480 @@
       <c r="Q66">
         <f t="shared" si="10"/>
         <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="3:17" ht="30">
+      <c r="C71" s="19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="72" spans="3:17" ht="16" thickBot="1"/>
+    <row r="73" spans="3:17" ht="16" thickBot="1">
+      <c r="C73" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D73" s="3">
+        <v>0</v>
+      </c>
+      <c r="F73" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="G73" s="21"/>
+      <c r="H73" s="21"/>
+      <c r="I73" s="21"/>
+      <c r="J73" s="21"/>
+      <c r="K73" s="21"/>
+      <c r="L73" s="21"/>
+      <c r="M73" s="21"/>
+    </row>
+    <row r="74" spans="3:17" ht="16" thickBot="1">
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="F74" s="21"/>
+      <c r="G74" s="21"/>
+      <c r="H74" s="21"/>
+      <c r="I74" s="21"/>
+      <c r="J74" s="21"/>
+      <c r="K74" s="21"/>
+      <c r="L74" s="21"/>
+      <c r="M74" s="21"/>
+    </row>
+    <row r="75" spans="3:17">
+      <c r="C75" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D75" s="3">
+        <v>1</v>
+      </c>
+      <c r="F75" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="G75" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="H75" s="21"/>
+      <c r="I75" s="21"/>
+      <c r="J75" s="21"/>
+      <c r="K75" s="21"/>
+      <c r="L75" s="21"/>
+      <c r="M75" s="21"/>
+    </row>
+    <row r="76" spans="3:17" ht="16" thickBot="1">
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="F76" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="G76" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="H76" s="21"/>
+      <c r="I76" s="21"/>
+      <c r="J76" s="21"/>
+      <c r="K76" s="21"/>
+      <c r="L76" s="21"/>
+      <c r="M76" s="21"/>
+    </row>
+    <row r="77" spans="3:17" ht="16" thickBot="1">
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="F77" s="21"/>
+      <c r="G77" s="21"/>
+      <c r="H77" s="21"/>
+      <c r="I77" s="21"/>
+      <c r="J77" s="21"/>
+      <c r="K77" s="21"/>
+      <c r="L77" s="21"/>
+      <c r="M77" s="21"/>
+    </row>
+    <row r="78" spans="3:17">
+      <c r="C78" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D78" s="3">
+        <v>2</v>
+      </c>
+      <c r="F78" s="42" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$78) &amp; "," &amp;ROW()-ROW( $F$78)</f>
+        <v>0,0</v>
+      </c>
+      <c r="G78" s="43" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$78) &amp; "," &amp;ROW()-ROW( $F$78)</f>
+        <v>1,0</v>
+      </c>
+      <c r="H78" s="46" t="str">
+        <f t="shared" ref="H78:I81" si="11" xml:space="preserve"> COLUMN()-COLUMN( $F$78) &amp; "," &amp;ROW()-ROW( $F$78)</f>
+        <v>2,0</v>
+      </c>
+      <c r="I78" s="47" t="str">
+        <f t="shared" si="11"/>
+        <v>3,0</v>
+      </c>
+      <c r="J78" s="21"/>
+      <c r="K78" s="21"/>
+      <c r="L78" s="21"/>
+      <c r="M78" s="21"/>
+    </row>
+    <row r="79" spans="3:17">
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="F79" s="44" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$78) &amp; "," &amp;ROW()-ROW( $F$78)</f>
+        <v>0,1</v>
+      </c>
+      <c r="G79" s="45" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$78) &amp; "," &amp;ROW()-ROW( $F$78)</f>
+        <v>1,1</v>
+      </c>
+      <c r="H79" s="48" t="str">
+        <f t="shared" si="11"/>
+        <v>2,1</v>
+      </c>
+      <c r="I79" s="49" t="str">
+        <f t="shared" si="11"/>
+        <v>3,1</v>
+      </c>
+      <c r="J79" s="21"/>
+      <c r="K79" s="21"/>
+      <c r="L79" s="21"/>
+      <c r="M79" s="21"/>
+    </row>
+    <row r="80" spans="3:17">
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="F80" s="50" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$78) &amp; "," &amp;ROW()-ROW( $F$78)</f>
+        <v>0,2</v>
+      </c>
+      <c r="G80" s="51" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$78) &amp; "," &amp;ROW()-ROW( $F$78)</f>
+        <v>1,2</v>
+      </c>
+      <c r="H80" s="54" t="str">
+        <f t="shared" si="11"/>
+        <v>2,2</v>
+      </c>
+      <c r="I80" s="55" t="str">
+        <f t="shared" si="11"/>
+        <v>3,2</v>
+      </c>
+      <c r="J80" s="21"/>
+      <c r="K80" s="21"/>
+      <c r="L80" s="21"/>
+      <c r="M80" s="21"/>
+    </row>
+    <row r="81" spans="3:13" ht="16" thickBot="1">
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="F81" s="52" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$78) &amp; "," &amp;ROW()-ROW( $F$78)</f>
+        <v>0,3</v>
+      </c>
+      <c r="G81" s="53" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$78) &amp; "," &amp;ROW()-ROW( $F$78)</f>
+        <v>1,3</v>
+      </c>
+      <c r="H81" s="56" t="str">
+        <f t="shared" si="11"/>
+        <v>2,3</v>
+      </c>
+      <c r="I81" s="57" t="str">
+        <f t="shared" si="11"/>
+        <v>3,3</v>
+      </c>
+      <c r="J81" s="21"/>
+      <c r="K81" s="21"/>
+      <c r="L81" s="21"/>
+      <c r="M81" s="21"/>
+    </row>
+    <row r="82" spans="3:13" ht="16" thickBot="1">
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="F82" s="21"/>
+      <c r="G82" s="21"/>
+      <c r="H82" s="21"/>
+      <c r="I82" s="21"/>
+      <c r="J82" s="21"/>
+      <c r="K82" s="21"/>
+      <c r="L82" s="21"/>
+      <c r="M82" s="21"/>
+    </row>
+    <row r="83" spans="3:13">
+      <c r="C83" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D83" s="3">
+        <v>3</v>
+      </c>
+      <c r="F83" s="23" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$83) &amp; "," &amp;ROW()-ROW( $F$83)</f>
+        <v>0,0</v>
+      </c>
+      <c r="G83" s="27" t="str">
+        <f t="shared" ref="G83:M90" si="12" xml:space="preserve"> COLUMN()-COLUMN( $F$83) &amp; "," &amp;ROW()-ROW( $F$83)</f>
+        <v>1,0</v>
+      </c>
+      <c r="H83" s="63" t="str">
+        <f t="shared" si="12"/>
+        <v>2,0</v>
+      </c>
+      <c r="I83" s="27" t="str">
+        <f t="shared" si="12"/>
+        <v>3,0</v>
+      </c>
+      <c r="J83" s="31" t="str">
+        <f t="shared" si="12"/>
+        <v>4,0</v>
+      </c>
+      <c r="K83" s="27" t="str">
+        <f t="shared" si="12"/>
+        <v>5,0</v>
+      </c>
+      <c r="L83" s="63" t="str">
+        <f t="shared" si="12"/>
+        <v>6,0</v>
+      </c>
+      <c r="M83" s="24" t="str">
+        <f t="shared" si="12"/>
+        <v>7,0</v>
+      </c>
+    </row>
+    <row r="84" spans="3:13">
+      <c r="F84" s="58" t="str">
+        <f t="shared" ref="F84:F90" si="13" xml:space="preserve"> COLUMN()-COLUMN( $F$83) &amp; "," &amp;ROW()-ROW( $F$83)</f>
+        <v>0,1</v>
+      </c>
+      <c r="G84" s="59" t="str">
+        <f t="shared" si="12"/>
+        <v>1,1</v>
+      </c>
+      <c r="H84" s="64" t="str">
+        <f t="shared" si="12"/>
+        <v>2,1</v>
+      </c>
+      <c r="I84" s="59" t="str">
+        <f t="shared" si="12"/>
+        <v>3,1</v>
+      </c>
+      <c r="J84" s="60" t="str">
+        <f t="shared" si="12"/>
+        <v>4,1</v>
+      </c>
+      <c r="K84" s="59" t="str">
+        <f t="shared" si="12"/>
+        <v>5,1</v>
+      </c>
+      <c r="L84" s="64" t="str">
+        <f t="shared" si="12"/>
+        <v>6,1</v>
+      </c>
+      <c r="M84" s="61" t="str">
+        <f t="shared" si="12"/>
+        <v>7,1</v>
+      </c>
+    </row>
+    <row r="85" spans="3:13">
+      <c r="F85" s="62" t="str">
+        <f t="shared" si="13"/>
+        <v>0,2</v>
+      </c>
+      <c r="G85" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>1,2</v>
+      </c>
+      <c r="H85" s="65" t="str">
+        <f t="shared" si="12"/>
+        <v>2,2</v>
+      </c>
+      <c r="I85" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>3,2</v>
+      </c>
+      <c r="J85" s="32" t="str">
+        <f t="shared" si="12"/>
+        <v>4,2</v>
+      </c>
+      <c r="K85" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>5,2</v>
+      </c>
+      <c r="L85" s="65" t="str">
+        <f t="shared" si="12"/>
+        <v>6,2</v>
+      </c>
+      <c r="M85" s="29" t="str">
+        <f t="shared" si="12"/>
+        <v>7,2</v>
+      </c>
+    </row>
+    <row r="86" spans="3:13">
+      <c r="F86" s="34" t="str">
+        <f t="shared" si="13"/>
+        <v>0,3</v>
+      </c>
+      <c r="G86" s="35" t="str">
+        <f t="shared" si="12"/>
+        <v>1,3</v>
+      </c>
+      <c r="H86" s="66" t="str">
+        <f t="shared" si="12"/>
+        <v>2,3</v>
+      </c>
+      <c r="I86" s="35" t="str">
+        <f t="shared" si="12"/>
+        <v>3,3</v>
+      </c>
+      <c r="J86" s="36" t="str">
+        <f t="shared" si="12"/>
+        <v>4,3</v>
+      </c>
+      <c r="K86" s="35" t="str">
+        <f t="shared" si="12"/>
+        <v>5,3</v>
+      </c>
+      <c r="L86" s="66" t="str">
+        <f t="shared" si="12"/>
+        <v>6,3</v>
+      </c>
+      <c r="M86" s="37" t="str">
+        <f t="shared" si="12"/>
+        <v>7,3</v>
+      </c>
+    </row>
+    <row r="87" spans="3:13">
+      <c r="F87" s="28" t="str">
+        <f t="shared" si="13"/>
+        <v>0,4</v>
+      </c>
+      <c r="G87" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>1,4</v>
+      </c>
+      <c r="H87" s="65" t="str">
+        <f t="shared" si="12"/>
+        <v>2,4</v>
+      </c>
+      <c r="I87" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>3,4</v>
+      </c>
+      <c r="J87" s="32" t="str">
+        <f t="shared" si="12"/>
+        <v>4,4</v>
+      </c>
+      <c r="K87" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>5,4</v>
+      </c>
+      <c r="L87" s="65" t="str">
+        <f t="shared" si="12"/>
+        <v>6,4</v>
+      </c>
+      <c r="M87" s="29" t="str">
+        <f t="shared" si="12"/>
+        <v>7,4</v>
+      </c>
+    </row>
+    <row r="88" spans="3:13">
+      <c r="F88" s="58" t="str">
+        <f t="shared" si="13"/>
+        <v>0,5</v>
+      </c>
+      <c r="G88" s="59" t="str">
+        <f t="shared" si="12"/>
+        <v>1,5</v>
+      </c>
+      <c r="H88" s="64" t="str">
+        <f t="shared" si="12"/>
+        <v>2,5</v>
+      </c>
+      <c r="I88" s="59" t="str">
+        <f t="shared" si="12"/>
+        <v>3,5</v>
+      </c>
+      <c r="J88" s="60" t="str">
+        <f t="shared" si="12"/>
+        <v>4,5</v>
+      </c>
+      <c r="K88" s="59" t="str">
+        <f t="shared" si="12"/>
+        <v>5,5</v>
+      </c>
+      <c r="L88" s="64" t="str">
+        <f t="shared" si="12"/>
+        <v>6,5</v>
+      </c>
+      <c r="M88" s="61" t="str">
+        <f t="shared" si="12"/>
+        <v>7,5</v>
+      </c>
+    </row>
+    <row r="89" spans="3:13">
+      <c r="F89" s="28" t="str">
+        <f t="shared" si="13"/>
+        <v>0,6</v>
+      </c>
+      <c r="G89" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>1,6</v>
+      </c>
+      <c r="H89" s="65" t="str">
+        <f t="shared" si="12"/>
+        <v>2,6</v>
+      </c>
+      <c r="I89" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>3,6</v>
+      </c>
+      <c r="J89" s="32" t="str">
+        <f t="shared" si="12"/>
+        <v>4,6</v>
+      </c>
+      <c r="K89" s="22" t="str">
+        <f t="shared" si="12"/>
+        <v>5,6</v>
+      </c>
+      <c r="L89" s="65" t="str">
+        <f t="shared" si="12"/>
+        <v>6,6</v>
+      </c>
+      <c r="M89" s="29" t="str">
+        <f t="shared" si="12"/>
+        <v>7,6</v>
+      </c>
+    </row>
+    <row r="90" spans="3:13" ht="16" thickBot="1">
+      <c r="F90" s="25" t="str">
+        <f t="shared" si="13"/>
+        <v>0,7</v>
+      </c>
+      <c r="G90" s="30" t="str">
+        <f t="shared" si="12"/>
+        <v>1,7</v>
+      </c>
+      <c r="H90" s="67" t="str">
+        <f t="shared" si="12"/>
+        <v>2,7</v>
+      </c>
+      <c r="I90" s="30" t="str">
+        <f t="shared" si="12"/>
+        <v>3,7</v>
+      </c>
+      <c r="J90" s="33" t="str">
+        <f t="shared" si="12"/>
+        <v>4,7</v>
+      </c>
+      <c r="K90" s="30" t="str">
+        <f t="shared" si="12"/>
+        <v>5,7</v>
+      </c>
+      <c r="L90" s="67" t="str">
+        <f t="shared" si="12"/>
+        <v>6,7</v>
+      </c>
+      <c r="M90" s="26" t="str">
+        <f t="shared" si="12"/>
+        <v>7,7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First attempt at zooming to edit
</commit_message>
<xml_diff>
--- a/burner/docs/zoomcalcs.xlsx
+++ b/burner/docs/zoomcalcs.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="54600" yWindow="640" windowWidth="42080" windowHeight="26820" tabRatio="500"/>
+    <workbookView xWindow="22420" yWindow="0" windowWidth="27040" windowHeight="27500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Zoom Calcs" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="110">
   <si>
     <t>0,0</t>
   </si>
@@ -133,13 +134,229 @@
   </si>
   <si>
     <t xml:space="preserve">Invalidation Areas </t>
+  </si>
+  <si>
+    <t>Copying</t>
+  </si>
+  <si>
+    <t>Copying between 2 different levels</t>
+  </si>
+  <si>
+    <t>Source Level</t>
+  </si>
+  <si>
+    <t>DestinationLevel</t>
+  </si>
+  <si>
+    <t>startX</t>
+  </si>
+  <si>
+    <t>destX</t>
+  </si>
+  <si>
+    <t>destTileX</t>
+  </si>
+  <si>
+    <t>srcTileX</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>2,0</t>
+  </si>
+  <si>
+    <t>3,0</t>
+  </si>
+  <si>
+    <t>2,1</t>
+  </si>
+  <si>
+    <t>3,1</t>
+  </si>
+  <si>
+    <t>0,2</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>2,2</t>
+  </si>
+  <si>
+    <t>3,2</t>
+  </si>
+  <si>
+    <t>0,3</t>
+  </si>
+  <si>
+    <t>1,3</t>
+  </si>
+  <si>
+    <t>2,3</t>
+  </si>
+  <si>
+    <t>3,3</t>
+  </si>
+  <si>
+    <t>4,0</t>
+  </si>
+  <si>
+    <t>5,0</t>
+  </si>
+  <si>
+    <t>6,0</t>
+  </si>
+  <si>
+    <t>7,0</t>
+  </si>
+  <si>
+    <t>4,1</t>
+  </si>
+  <si>
+    <t>5,1</t>
+  </si>
+  <si>
+    <t>6,1</t>
+  </si>
+  <si>
+    <t>7,1</t>
+  </si>
+  <si>
+    <t>4,2</t>
+  </si>
+  <si>
+    <t>5,2</t>
+  </si>
+  <si>
+    <t>6,2</t>
+  </si>
+  <si>
+    <t>7,2</t>
+  </si>
+  <si>
+    <t>4,3</t>
+  </si>
+  <si>
+    <t>5,3</t>
+  </si>
+  <si>
+    <t>6,3</t>
+  </si>
+  <si>
+    <t>7,3</t>
+  </si>
+  <si>
+    <t>0,4</t>
+  </si>
+  <si>
+    <t>1,4</t>
+  </si>
+  <si>
+    <t>2,4</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>4,4</t>
+  </si>
+  <si>
+    <t>5,4</t>
+  </si>
+  <si>
+    <t>6,4</t>
+  </si>
+  <si>
+    <t>7,4</t>
+  </si>
+  <si>
+    <t>0,5</t>
+  </si>
+  <si>
+    <t>1,5</t>
+  </si>
+  <si>
+    <t>2,5</t>
+  </si>
+  <si>
+    <t>3,5</t>
+  </si>
+  <si>
+    <t>4,5</t>
+  </si>
+  <si>
+    <t>5,5</t>
+  </si>
+  <si>
+    <t>6,5</t>
+  </si>
+  <si>
+    <t>7,5</t>
+  </si>
+  <si>
+    <t>0,6</t>
+  </si>
+  <si>
+    <t>1,6</t>
+  </si>
+  <si>
+    <t>2,6</t>
+  </si>
+  <si>
+    <t>3,6</t>
+  </si>
+  <si>
+    <t>4,6</t>
+  </si>
+  <si>
+    <t>5,6</t>
+  </si>
+  <si>
+    <t>6,6</t>
+  </si>
+  <si>
+    <t>7,6</t>
+  </si>
+  <si>
+    <t>0,7</t>
+  </si>
+  <si>
+    <t>1,7</t>
+  </si>
+  <si>
+    <t>2,7</t>
+  </si>
+  <si>
+    <t>3,7</t>
+  </si>
+  <si>
+    <t>4,7</t>
+  </si>
+  <si>
+    <t>5,7</t>
+  </si>
+  <si>
+    <t>6,7</t>
+  </si>
+  <si>
+    <t>7,7</t>
+  </si>
+  <si>
+    <t>Copying a Layer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -213,6 +430,12 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -892,7 +1115,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -910,8 +1133,56 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -1084,8 +1355,21 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="51" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="65">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
     <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1094,6 +1378,30 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -1101,6 +1409,30 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -5988,6 +6320,71 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>469900</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>101600</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>22</xdr:col>
+          <xdr:colOff>381000</xdr:colOff>
+          <xdr:row>49</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="Picture 1"/>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+              <a:extLst>
+                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
+                  <a14:cameraTool cellRange="'Zoom Calcs'!$B$131:$V$171" spid="_x0000_s2058"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="1295400" y="1054100"/>
+              <a:ext cx="17246600" cy="8280400"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+            </a:solidFill>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd type="none" w="med" len="med"/>
+              <a:tailEnd type="none" w="med" len="med"/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6310,10 +6707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:X90"/>
+  <dimension ref="B2:X169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N78" sqref="N78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7345,19 +7742,19 @@
         <v>2</v>
       </c>
       <c r="F78" s="42" t="str">
-        <f xml:space="preserve"> COLUMN()-COLUMN( $F$78) &amp; "," &amp;ROW()-ROW( $F$78)</f>
+        <f t="shared" ref="F78:G81" si="11" xml:space="preserve"> COLUMN()-COLUMN( $F$78) &amp; "," &amp;ROW()-ROW( $F$78)</f>
         <v>0,0</v>
       </c>
       <c r="G78" s="43" t="str">
-        <f xml:space="preserve"> COLUMN()-COLUMN( $F$78) &amp; "," &amp;ROW()-ROW( $F$78)</f>
+        <f t="shared" si="11"/>
         <v>1,0</v>
       </c>
       <c r="H78" s="46" t="str">
-        <f t="shared" ref="H78:I81" si="11" xml:space="preserve"> COLUMN()-COLUMN( $F$78) &amp; "," &amp;ROW()-ROW( $F$78)</f>
+        <f t="shared" ref="H78:I81" si="12" xml:space="preserve"> COLUMN()-COLUMN( $F$78) &amp; "," &amp;ROW()-ROW( $F$78)</f>
         <v>2,0</v>
       </c>
       <c r="I78" s="47" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3,0</v>
       </c>
       <c r="J78" s="21"/>
@@ -7369,19 +7766,19 @@
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
       <c r="F79" s="44" t="str">
-        <f xml:space="preserve"> COLUMN()-COLUMN( $F$78) &amp; "," &amp;ROW()-ROW( $F$78)</f>
+        <f t="shared" si="11"/>
         <v>0,1</v>
       </c>
       <c r="G79" s="45" t="str">
-        <f xml:space="preserve"> COLUMN()-COLUMN( $F$78) &amp; "," &amp;ROW()-ROW( $F$78)</f>
+        <f t="shared" si="11"/>
         <v>1,1</v>
       </c>
       <c r="H79" s="48" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2,1</v>
       </c>
       <c r="I79" s="49" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3,1</v>
       </c>
       <c r="J79" s="21"/>
@@ -7393,19 +7790,19 @@
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
       <c r="F80" s="50" t="str">
-        <f xml:space="preserve"> COLUMN()-COLUMN( $F$78) &amp; "," &amp;ROW()-ROW( $F$78)</f>
+        <f t="shared" si="11"/>
         <v>0,2</v>
       </c>
       <c r="G80" s="51" t="str">
-        <f xml:space="preserve"> COLUMN()-COLUMN( $F$78) &amp; "," &amp;ROW()-ROW( $F$78)</f>
+        <f t="shared" si="11"/>
         <v>1,2</v>
       </c>
       <c r="H80" s="54" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2,2</v>
       </c>
       <c r="I80" s="55" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3,2</v>
       </c>
       <c r="J80" s="21"/>
@@ -7417,19 +7814,19 @@
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
       <c r="F81" s="52" t="str">
-        <f xml:space="preserve"> COLUMN()-COLUMN( $F$78) &amp; "," &amp;ROW()-ROW( $F$78)</f>
+        <f t="shared" si="11"/>
         <v>0,3</v>
       </c>
       <c r="G81" s="53" t="str">
-        <f xml:space="preserve"> COLUMN()-COLUMN( $F$78) &amp; "," &amp;ROW()-ROW( $F$78)</f>
+        <f t="shared" si="11"/>
         <v>1,3</v>
       </c>
       <c r="H81" s="56" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2,3</v>
       </c>
       <c r="I81" s="57" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3,3</v>
       </c>
       <c r="J81" s="21"/>
@@ -7461,270 +7858,2036 @@
         <v>0,0</v>
       </c>
       <c r="G83" s="27" t="str">
-        <f t="shared" ref="G83:M90" si="12" xml:space="preserve"> COLUMN()-COLUMN( $F$83) &amp; "," &amp;ROW()-ROW( $F$83)</f>
+        <f t="shared" ref="G83:M90" si="13" xml:space="preserve"> COLUMN()-COLUMN( $F$83) &amp; "," &amp;ROW()-ROW( $F$83)</f>
         <v>1,0</v>
       </c>
       <c r="H83" s="63" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2,0</v>
       </c>
       <c r="I83" s="27" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3,0</v>
       </c>
       <c r="J83" s="31" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4,0</v>
       </c>
       <c r="K83" s="27" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5,0</v>
       </c>
       <c r="L83" s="63" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6,0</v>
       </c>
       <c r="M83" s="24" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7,0</v>
       </c>
     </row>
     <row r="84" spans="3:13">
       <c r="F84" s="58" t="str">
-        <f t="shared" ref="F84:F90" si="13" xml:space="preserve"> COLUMN()-COLUMN( $F$83) &amp; "," &amp;ROW()-ROW( $F$83)</f>
+        <f t="shared" ref="F84:F90" si="14" xml:space="preserve"> COLUMN()-COLUMN( $F$83) &amp; "," &amp;ROW()-ROW( $F$83)</f>
         <v>0,1</v>
       </c>
       <c r="G84" s="59" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1,1</v>
       </c>
       <c r="H84" s="64" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2,1</v>
       </c>
       <c r="I84" s="59" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3,1</v>
       </c>
       <c r="J84" s="60" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4,1</v>
       </c>
       <c r="K84" s="59" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5,1</v>
       </c>
       <c r="L84" s="64" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6,1</v>
       </c>
       <c r="M84" s="61" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7,1</v>
       </c>
     </row>
     <row r="85" spans="3:13">
       <c r="F85" s="62" t="str">
+        <f t="shared" si="14"/>
+        <v>0,2</v>
+      </c>
+      <c r="G85" s="22" t="str">
         <f t="shared" si="13"/>
-        <v>0,2</v>
-      </c>
-      <c r="G85" s="22" t="str">
-        <f t="shared" si="12"/>
         <v>1,2</v>
       </c>
       <c r="H85" s="65" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2,2</v>
       </c>
       <c r="I85" s="22" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3,2</v>
       </c>
       <c r="J85" s="32" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4,2</v>
       </c>
       <c r="K85" s="22" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5,2</v>
       </c>
       <c r="L85" s="65" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6,2</v>
       </c>
       <c r="M85" s="29" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7,2</v>
       </c>
     </row>
     <row r="86" spans="3:13">
       <c r="F86" s="34" t="str">
+        <f t="shared" si="14"/>
+        <v>0,3</v>
+      </c>
+      <c r="G86" s="35" t="str">
         <f t="shared" si="13"/>
-        <v>0,3</v>
-      </c>
-      <c r="G86" s="35" t="str">
-        <f t="shared" si="12"/>
         <v>1,3</v>
       </c>
       <c r="H86" s="66" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2,3</v>
       </c>
       <c r="I86" s="35" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3,3</v>
       </c>
       <c r="J86" s="36" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4,3</v>
       </c>
       <c r="K86" s="35" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5,3</v>
       </c>
       <c r="L86" s="66" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6,3</v>
       </c>
       <c r="M86" s="37" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7,3</v>
       </c>
     </row>
     <row r="87" spans="3:13">
       <c r="F87" s="28" t="str">
+        <f t="shared" si="14"/>
+        <v>0,4</v>
+      </c>
+      <c r="G87" s="22" t="str">
         <f t="shared" si="13"/>
-        <v>0,4</v>
-      </c>
-      <c r="G87" s="22" t="str">
-        <f t="shared" si="12"/>
         <v>1,4</v>
       </c>
       <c r="H87" s="65" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2,4</v>
       </c>
       <c r="I87" s="22" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3,4</v>
       </c>
       <c r="J87" s="32" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4,4</v>
       </c>
       <c r="K87" s="22" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5,4</v>
       </c>
       <c r="L87" s="65" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6,4</v>
       </c>
       <c r="M87" s="29" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7,4</v>
       </c>
     </row>
     <row r="88" spans="3:13">
       <c r="F88" s="58" t="str">
+        <f t="shared" si="14"/>
+        <v>0,5</v>
+      </c>
+      <c r="G88" s="59" t="str">
         <f t="shared" si="13"/>
-        <v>0,5</v>
-      </c>
-      <c r="G88" s="59" t="str">
-        <f t="shared" si="12"/>
         <v>1,5</v>
       </c>
       <c r="H88" s="64" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2,5</v>
       </c>
       <c r="I88" s="59" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3,5</v>
       </c>
       <c r="J88" s="60" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4,5</v>
       </c>
       <c r="K88" s="59" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5,5</v>
       </c>
       <c r="L88" s="64" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6,5</v>
       </c>
       <c r="M88" s="61" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7,5</v>
       </c>
     </row>
     <row r="89" spans="3:13">
       <c r="F89" s="28" t="str">
+        <f t="shared" si="14"/>
+        <v>0,6</v>
+      </c>
+      <c r="G89" s="22" t="str">
         <f t="shared" si="13"/>
-        <v>0,6</v>
-      </c>
-      <c r="G89" s="22" t="str">
-        <f t="shared" si="12"/>
         <v>1,6</v>
       </c>
       <c r="H89" s="65" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2,6</v>
       </c>
       <c r="I89" s="22" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3,6</v>
       </c>
       <c r="J89" s="32" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4,6</v>
       </c>
       <c r="K89" s="22" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5,6</v>
       </c>
       <c r="L89" s="65" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6,6</v>
       </c>
       <c r="M89" s="29" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7,6</v>
       </c>
     </row>
     <row r="90" spans="3:13" ht="16" thickBot="1">
       <c r="F90" s="25" t="str">
+        <f t="shared" si="14"/>
+        <v>0,7</v>
+      </c>
+      <c r="G90" s="30" t="str">
         <f t="shared" si="13"/>
+        <v>1,7</v>
+      </c>
+      <c r="H90" s="67" t="str">
+        <f t="shared" si="13"/>
+        <v>2,7</v>
+      </c>
+      <c r="I90" s="30" t="str">
+        <f t="shared" si="13"/>
+        <v>3,7</v>
+      </c>
+      <c r="J90" s="33" t="str">
+        <f t="shared" si="13"/>
+        <v>4,7</v>
+      </c>
+      <c r="K90" s="30" t="str">
+        <f t="shared" si="13"/>
+        <v>5,7</v>
+      </c>
+      <c r="L90" s="67" t="str">
+        <f t="shared" si="13"/>
+        <v>6,7</v>
+      </c>
+      <c r="M90" s="26" t="str">
+        <f t="shared" si="13"/>
+        <v>7,7</v>
+      </c>
+    </row>
+    <row r="96" spans="3:13" ht="30">
+      <c r="C96" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="99" spans="3:18">
+      <c r="C99" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="101" spans="3:18">
+      <c r="C101" t="s">
+        <v>40</v>
+      </c>
+      <c r="E101" t="s">
+        <v>41</v>
+      </c>
+      <c r="G101" t="s">
+        <v>42</v>
+      </c>
+      <c r="H101" t="s">
+        <v>43</v>
+      </c>
+      <c r="J101" t="s">
+        <v>45</v>
+      </c>
+      <c r="K101" t="s">
+        <v>44</v>
+      </c>
+      <c r="M101" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N101" t="s">
+        <v>46</v>
+      </c>
+      <c r="O101" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="102" spans="3:18">
+      <c r="M102" s="1">
+        <v>1</v>
+      </c>
+      <c r="N102">
+        <v>1</v>
+      </c>
+      <c r="O102">
+        <v>0</v>
+      </c>
+      <c r="Q102">
+        <v>2</v>
+      </c>
+      <c r="R102">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="3:18">
+      <c r="C103">
+        <v>5</v>
+      </c>
+      <c r="E103">
+        <v>5</v>
+      </c>
+      <c r="G103">
+        <v>5</v>
+      </c>
+      <c r="H103">
+        <v>8</v>
+      </c>
+      <c r="I103" s="68"/>
+      <c r="J103">
+        <v>10</v>
+      </c>
+      <c r="K103">
+        <v>13</v>
+      </c>
+      <c r="M103" s="1"/>
+      <c r="Q103">
+        <v>3</v>
+      </c>
+      <c r="R103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="3:18">
+      <c r="I104" s="68"/>
+      <c r="M104" s="1"/>
+    </row>
+    <row r="105" spans="3:18">
+      <c r="M105" s="1"/>
+      <c r="Q105">
+        <v>2</v>
+      </c>
+      <c r="R105">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="3:18">
+      <c r="C106">
+        <v>5</v>
+      </c>
+      <c r="E106">
+        <v>6</v>
+      </c>
+      <c r="G106">
+        <v>5</v>
+      </c>
+      <c r="H106">
+        <v>8</v>
+      </c>
+      <c r="J106">
+        <v>10</v>
+      </c>
+      <c r="M106" s="1"/>
+      <c r="Q106">
+        <v>3</v>
+      </c>
+      <c r="R106">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="3:18">
+      <c r="M107" s="1"/>
+    </row>
+    <row r="108" spans="3:18">
+      <c r="M108" s="1"/>
+    </row>
+    <row r="109" spans="3:18">
+      <c r="M109" s="1">
+        <v>2</v>
+      </c>
+      <c r="N109">
+        <v>2</v>
+      </c>
+      <c r="O109">
+        <v>2</v>
+      </c>
+      <c r="Q109">
+        <v>4</v>
+      </c>
+      <c r="R109">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="3:18">
+      <c r="M110" s="1"/>
+      <c r="Q110">
+        <v>5</v>
+      </c>
+      <c r="R110">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="3:18">
+      <c r="M111" s="1"/>
+      <c r="Q111">
+        <v>6</v>
+      </c>
+      <c r="R111">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="3:18">
+      <c r="M112" s="1"/>
+      <c r="Q112">
+        <v>7</v>
+      </c>
+      <c r="R112">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="13:18">
+      <c r="M113" s="1"/>
+    </row>
+    <row r="114" spans="13:18">
+      <c r="M114" s="1">
+        <v>2</v>
+      </c>
+      <c r="N114">
+        <v>3</v>
+      </c>
+      <c r="O114">
+        <v>2</v>
+      </c>
+      <c r="Q114">
+        <v>4</v>
+      </c>
+      <c r="R114">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="13:18">
+      <c r="M115" s="1"/>
+      <c r="Q115">
+        <v>5</v>
+      </c>
+      <c r="R115">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="13:18">
+      <c r="M116" s="1"/>
+      <c r="Q116">
+        <v>6</v>
+      </c>
+      <c r="R116">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="13:18">
+      <c r="M117" s="1"/>
+      <c r="Q117">
+        <v>7</v>
+      </c>
+      <c r="R117">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="13:18">
+      <c r="M118" s="1"/>
+    </row>
+    <row r="119" spans="13:18">
+      <c r="M119" s="1">
+        <v>2</v>
+      </c>
+      <c r="N119">
+        <v>2</v>
+      </c>
+      <c r="O119">
+        <v>3</v>
+      </c>
+      <c r="Q119">
+        <v>4</v>
+      </c>
+      <c r="R119">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120" spans="13:18">
+      <c r="M120" s="1"/>
+      <c r="Q120">
+        <v>5</v>
+      </c>
+      <c r="R120">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121" spans="13:18">
+      <c r="M121" s="1"/>
+      <c r="Q121">
+        <v>6</v>
+      </c>
+      <c r="R121">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="13:18">
+      <c r="M122" s="1"/>
+      <c r="Q122">
+        <v>7</v>
+      </c>
+      <c r="R122">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="123" spans="13:18">
+      <c r="M123" s="1"/>
+    </row>
+    <row r="124" spans="13:18">
+      <c r="M124" s="1">
+        <v>2</v>
+      </c>
+      <c r="N124">
+        <v>3</v>
+      </c>
+      <c r="O124">
+        <v>3</v>
+      </c>
+      <c r="Q124">
+        <v>4</v>
+      </c>
+      <c r="R124">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="125" spans="13:18">
+      <c r="Q125">
+        <v>5</v>
+      </c>
+      <c r="R125">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="126" spans="13:18">
+      <c r="Q126">
+        <v>6</v>
+      </c>
+      <c r="R126">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="127" spans="13:18">
+      <c r="Q127">
+        <v>7</v>
+      </c>
+      <c r="R127">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="132" spans="3:13" ht="30">
+      <c r="C132" s="19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="133" spans="3:13" ht="16" thickBot="1"/>
+    <row r="134" spans="3:13" ht="16" thickBot="1">
+      <c r="C134" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D134" s="3">
+        <v>0</v>
+      </c>
+      <c r="F134" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="G134" s="21"/>
+      <c r="H134" s="21"/>
+      <c r="I134" s="21"/>
+      <c r="J134" s="21"/>
+      <c r="K134" s="21"/>
+      <c r="L134" s="21"/>
+      <c r="M134" s="21"/>
+    </row>
+    <row r="135" spans="3:13" ht="16" thickBot="1">
+      <c r="C135" s="3"/>
+      <c r="D135" s="3"/>
+      <c r="F135" s="21"/>
+      <c r="G135" s="21"/>
+      <c r="H135" s="21"/>
+      <c r="I135" s="21"/>
+      <c r="J135" s="21"/>
+      <c r="K135" s="21"/>
+      <c r="L135" s="21"/>
+      <c r="M135" s="21"/>
+    </row>
+    <row r="136" spans="3:13">
+      <c r="C136" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D136" s="3">
+        <v>1</v>
+      </c>
+      <c r="F136" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="G136" s="71" t="s">
+        <v>1</v>
+      </c>
+      <c r="H136" s="21"/>
+      <c r="I136" s="21"/>
+      <c r="J136" s="21"/>
+      <c r="K136" s="21"/>
+      <c r="L136" s="21"/>
+      <c r="M136" s="21"/>
+    </row>
+    <row r="137" spans="3:13" ht="16" thickBot="1">
+      <c r="C137" s="3"/>
+      <c r="D137" s="3"/>
+      <c r="F137" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="G137" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="H137" s="21"/>
+      <c r="I137" s="21"/>
+      <c r="J137" s="21"/>
+      <c r="K137" s="21"/>
+      <c r="L137" s="21"/>
+      <c r="M137" s="21"/>
+    </row>
+    <row r="138" spans="3:13" ht="16" thickBot="1">
+      <c r="C138" s="3"/>
+      <c r="D138" s="3"/>
+      <c r="F138" s="21"/>
+      <c r="G138" s="21"/>
+      <c r="H138" s="21"/>
+      <c r="I138" s="21"/>
+      <c r="J138" s="21"/>
+      <c r="K138" s="21"/>
+      <c r="L138" s="21"/>
+      <c r="M138" s="21"/>
+    </row>
+    <row r="139" spans="3:13" ht="17" thickTop="1" thickBot="1">
+      <c r="C139" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D139" s="3">
+        <v>2</v>
+      </c>
+      <c r="F139" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="G139" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="H139" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="I139" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J139" s="21"/>
+      <c r="K139" s="21"/>
+      <c r="L139" s="21"/>
+      <c r="M139" s="21"/>
+    </row>
+    <row r="140" spans="3:13" ht="17" thickTop="1" thickBot="1">
+      <c r="C140" s="3"/>
+      <c r="D140" s="3"/>
+      <c r="F140" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="G140" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="H140" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="I140" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J140" s="21"/>
+      <c r="K140" s="21"/>
+      <c r="L140" s="21"/>
+      <c r="M140" s="21"/>
+    </row>
+    <row r="141" spans="3:13" ht="16" thickTop="1">
+      <c r="C141" s="3"/>
+      <c r="D141" s="3"/>
+      <c r="F141" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="G141" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="H141" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="I141" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="J141" s="21"/>
+      <c r="K141" s="21"/>
+      <c r="L141" s="21"/>
+      <c r="M141" s="21"/>
+    </row>
+    <row r="142" spans="3:13" ht="16" thickBot="1">
+      <c r="C142" s="3"/>
+      <c r="D142" s="3"/>
+      <c r="F142" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="G142" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="H142" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="I142" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="J142" s="21"/>
+      <c r="K142" s="21"/>
+      <c r="L142" s="21"/>
+      <c r="M142" s="21"/>
+    </row>
+    <row r="143" spans="3:13" ht="16" thickBot="1">
+      <c r="C143" s="3"/>
+      <c r="D143" s="3"/>
+      <c r="F143" s="21"/>
+      <c r="G143" s="21"/>
+      <c r="H143" s="21"/>
+      <c r="I143" s="21"/>
+      <c r="J143" s="21"/>
+      <c r="K143" s="21"/>
+      <c r="L143" s="21"/>
+      <c r="M143" s="21"/>
+    </row>
+    <row r="144" spans="3:13">
+      <c r="C144" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D144" s="3">
+        <v>3</v>
+      </c>
+      <c r="F144" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="G144" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="H144" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="I144" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="J144" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="K144" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="L144" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="M144" s="24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="145" spans="3:21">
+      <c r="F145" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="G145" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="H145" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="I145" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="J145" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="K145" s="59" t="s">
+        <v>66</v>
+      </c>
+      <c r="L145" s="64" t="s">
+        <v>67</v>
+      </c>
+      <c r="M145" s="61" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="146" spans="3:21">
+      <c r="F146" s="62" t="s">
+        <v>53</v>
+      </c>
+      <c r="G146" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="H146" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="I146" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="J146" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="K146" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="L146" s="65" t="s">
+        <v>71</v>
+      </c>
+      <c r="M146" s="29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="147" spans="3:21">
+      <c r="F147" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="G147" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="H147" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="I147" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="J147" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="K147" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="L147" s="66" t="s">
+        <v>75</v>
+      </c>
+      <c r="M147" s="37" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="148" spans="3:21">
+      <c r="F148" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="G148" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="H148" s="65" t="s">
+        <v>79</v>
+      </c>
+      <c r="I148" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="J148" s="69" t="s">
+        <v>81</v>
+      </c>
+      <c r="K148" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="L148" s="65" t="s">
+        <v>83</v>
+      </c>
+      <c r="M148" s="29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="149" spans="3:21">
+      <c r="F149" s="58" t="s">
+        <v>85</v>
+      </c>
+      <c r="G149" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="H149" s="64" t="s">
+        <v>87</v>
+      </c>
+      <c r="I149" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="J149" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="K149" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="L149" s="64" t="s">
+        <v>91</v>
+      </c>
+      <c r="M149" s="61" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="150" spans="3:21">
+      <c r="F150" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="G150" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="H150" s="65" t="s">
+        <v>95</v>
+      </c>
+      <c r="I150" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="J150" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="K150" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="L150" s="65" t="s">
+        <v>99</v>
+      </c>
+      <c r="M150" s="29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="151" spans="3:21" ht="16" thickBot="1">
+      <c r="F151" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="G151" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="H151" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="I151" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="J151" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="K151" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="L151" s="67" t="s">
+        <v>107</v>
+      </c>
+      <c r="M151" s="26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="153" spans="3:21" ht="16" thickBot="1"/>
+    <row r="154" spans="3:21">
+      <c r="C154" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D154" s="3">
+        <v>4</v>
+      </c>
+      <c r="F154" s="23" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$154) &amp; "," &amp;ROW()-ROW( $F$154)</f>
+        <v>0,0</v>
+      </c>
+      <c r="G154" s="27" t="str">
+        <f t="shared" ref="G154:U169" si="15" xml:space="preserve"> COLUMN()-COLUMN( $F$154) &amp; "," &amp;ROW()-ROW( $F$154)</f>
+        <v>1,0</v>
+      </c>
+      <c r="H154" s="63" t="str">
+        <f t="shared" si="15"/>
+        <v>2,0</v>
+      </c>
+      <c r="I154" s="27" t="str">
+        <f t="shared" si="15"/>
+        <v>3,0</v>
+      </c>
+      <c r="J154" s="31" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$154) &amp; "," &amp;ROW()-ROW( $F$154)</f>
+        <v>4,0</v>
+      </c>
+      <c r="K154" s="27" t="str">
+        <f t="shared" si="15"/>
+        <v>5,0</v>
+      </c>
+      <c r="L154" s="63" t="str">
+        <f t="shared" si="15"/>
+        <v>6,0</v>
+      </c>
+      <c r="M154" s="24" t="str">
+        <f t="shared" si="15"/>
+        <v>7,0</v>
+      </c>
+      <c r="N154" s="23" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$154) &amp; "," &amp;ROW()-ROW( $F$154)</f>
+        <v>8,0</v>
+      </c>
+      <c r="O154" s="27" t="str">
+        <f t="shared" si="15"/>
+        <v>9,0</v>
+      </c>
+      <c r="P154" s="63" t="str">
+        <f t="shared" si="15"/>
+        <v>10,0</v>
+      </c>
+      <c r="Q154" s="27" t="str">
+        <f t="shared" si="15"/>
+        <v>11,0</v>
+      </c>
+      <c r="R154" s="31" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$154) &amp; "," &amp;ROW()-ROW( $F$154)</f>
+        <v>12,0</v>
+      </c>
+      <c r="S154" s="27" t="str">
+        <f t="shared" si="15"/>
+        <v>13,0</v>
+      </c>
+      <c r="T154" s="63" t="str">
+        <f t="shared" si="15"/>
+        <v>14,0</v>
+      </c>
+      <c r="U154" s="24" t="str">
+        <f t="shared" si="15"/>
+        <v>15,0</v>
+      </c>
+    </row>
+    <row r="155" spans="3:21">
+      <c r="F155" s="58" t="str">
+        <f t="shared" ref="F155:F169" si="16" xml:space="preserve"> COLUMN()-COLUMN( $F$154) &amp; "," &amp;ROW()-ROW( $F$154)</f>
+        <v>0,1</v>
+      </c>
+      <c r="G155" s="59" t="str">
+        <f t="shared" si="15"/>
+        <v>1,1</v>
+      </c>
+      <c r="H155" s="64" t="str">
+        <f t="shared" si="15"/>
+        <v>2,1</v>
+      </c>
+      <c r="I155" s="59" t="str">
+        <f t="shared" si="15"/>
+        <v>3,1</v>
+      </c>
+      <c r="J155" s="60" t="str">
+        <f t="shared" si="15"/>
+        <v>4,1</v>
+      </c>
+      <c r="K155" s="59" t="str">
+        <f t="shared" si="15"/>
+        <v>5,1</v>
+      </c>
+      <c r="L155" s="64" t="str">
+        <f t="shared" si="15"/>
+        <v>6,1</v>
+      </c>
+      <c r="M155" s="61" t="str">
+        <f t="shared" si="15"/>
+        <v>7,1</v>
+      </c>
+      <c r="N155" s="58" t="str">
+        <f t="shared" si="15"/>
+        <v>8,1</v>
+      </c>
+      <c r="O155" s="59" t="str">
+        <f t="shared" si="15"/>
+        <v>9,1</v>
+      </c>
+      <c r="P155" s="64" t="str">
+        <f t="shared" si="15"/>
+        <v>10,1</v>
+      </c>
+      <c r="Q155" s="59" t="str">
+        <f t="shared" si="15"/>
+        <v>11,1</v>
+      </c>
+      <c r="R155" s="60" t="str">
+        <f t="shared" si="15"/>
+        <v>12,1</v>
+      </c>
+      <c r="S155" s="59" t="str">
+        <f t="shared" si="15"/>
+        <v>13,1</v>
+      </c>
+      <c r="T155" s="64" t="str">
+        <f t="shared" si="15"/>
+        <v>14,1</v>
+      </c>
+      <c r="U155" s="61" t="str">
+        <f t="shared" si="15"/>
+        <v>15,1</v>
+      </c>
+    </row>
+    <row r="156" spans="3:21">
+      <c r="F156" s="62" t="str">
+        <f t="shared" si="16"/>
+        <v>0,2</v>
+      </c>
+      <c r="G156" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>1,2</v>
+      </c>
+      <c r="H156" s="65" t="str">
+        <f t="shared" si="15"/>
+        <v>2,2</v>
+      </c>
+      <c r="I156" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>3,2</v>
+      </c>
+      <c r="J156" s="32" t="str">
+        <f t="shared" si="15"/>
+        <v>4,2</v>
+      </c>
+      <c r="K156" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>5,2</v>
+      </c>
+      <c r="L156" s="65" t="str">
+        <f t="shared" si="15"/>
+        <v>6,2</v>
+      </c>
+      <c r="M156" s="29" t="str">
+        <f t="shared" si="15"/>
+        <v>7,2</v>
+      </c>
+      <c r="N156" s="62" t="str">
+        <f t="shared" si="15"/>
+        <v>8,2</v>
+      </c>
+      <c r="O156" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>9,2</v>
+      </c>
+      <c r="P156" s="65" t="str">
+        <f t="shared" si="15"/>
+        <v>10,2</v>
+      </c>
+      <c r="Q156" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>11,2</v>
+      </c>
+      <c r="R156" s="32" t="str">
+        <f t="shared" si="15"/>
+        <v>12,2</v>
+      </c>
+      <c r="S156" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>13,2</v>
+      </c>
+      <c r="T156" s="65" t="str">
+        <f t="shared" si="15"/>
+        <v>14,2</v>
+      </c>
+      <c r="U156" s="29" t="str">
+        <f t="shared" si="15"/>
+        <v>15,2</v>
+      </c>
+    </row>
+    <row r="157" spans="3:21">
+      <c r="F157" s="34" t="str">
+        <f t="shared" si="16"/>
+        <v>0,3</v>
+      </c>
+      <c r="G157" s="35" t="str">
+        <f t="shared" si="15"/>
+        <v>1,3</v>
+      </c>
+      <c r="H157" s="66" t="str">
+        <f t="shared" si="15"/>
+        <v>2,3</v>
+      </c>
+      <c r="I157" s="35" t="str">
+        <f t="shared" si="15"/>
+        <v>3,3</v>
+      </c>
+      <c r="J157" s="36" t="str">
+        <f t="shared" si="15"/>
+        <v>4,3</v>
+      </c>
+      <c r="K157" s="35" t="str">
+        <f t="shared" si="15"/>
+        <v>5,3</v>
+      </c>
+      <c r="L157" s="66" t="str">
+        <f t="shared" si="15"/>
+        <v>6,3</v>
+      </c>
+      <c r="M157" s="37" t="str">
+        <f t="shared" si="15"/>
+        <v>7,3</v>
+      </c>
+      <c r="N157" s="34" t="str">
+        <f t="shared" si="15"/>
+        <v>8,3</v>
+      </c>
+      <c r="O157" s="35" t="str">
+        <f t="shared" si="15"/>
+        <v>9,3</v>
+      </c>
+      <c r="P157" s="66" t="str">
+        <f t="shared" si="15"/>
+        <v>10,3</v>
+      </c>
+      <c r="Q157" s="35" t="str">
+        <f t="shared" si="15"/>
+        <v>11,3</v>
+      </c>
+      <c r="R157" s="36" t="str">
+        <f t="shared" si="15"/>
+        <v>12,3</v>
+      </c>
+      <c r="S157" s="35" t="str">
+        <f t="shared" si="15"/>
+        <v>13,3</v>
+      </c>
+      <c r="T157" s="66" t="str">
+        <f t="shared" si="15"/>
+        <v>14,3</v>
+      </c>
+      <c r="U157" s="37" t="str">
+        <f t="shared" si="15"/>
+        <v>15,3</v>
+      </c>
+    </row>
+    <row r="158" spans="3:21">
+      <c r="F158" s="28" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$154) &amp; "," &amp;ROW()-ROW( $F$154)</f>
+        <v>0,4</v>
+      </c>
+      <c r="G158" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>1,4</v>
+      </c>
+      <c r="H158" s="65" t="str">
+        <f t="shared" si="15"/>
+        <v>2,4</v>
+      </c>
+      <c r="I158" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>3,4</v>
+      </c>
+      <c r="J158" s="70" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$154) &amp; "," &amp;ROW()-ROW( $F$154)</f>
+        <v>4,4</v>
+      </c>
+      <c r="K158" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>5,4</v>
+      </c>
+      <c r="L158" s="65" t="str">
+        <f t="shared" si="15"/>
+        <v>6,4</v>
+      </c>
+      <c r="M158" s="29" t="str">
+        <f t="shared" si="15"/>
+        <v>7,4</v>
+      </c>
+      <c r="N158" s="28" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$154) &amp; "," &amp;ROW()-ROW( $F$154)</f>
+        <v>8,4</v>
+      </c>
+      <c r="O158" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>9,4</v>
+      </c>
+      <c r="P158" s="65" t="str">
+        <f t="shared" si="15"/>
+        <v>10,4</v>
+      </c>
+      <c r="Q158" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>11,4</v>
+      </c>
+      <c r="R158" s="70" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$154) &amp; "," &amp;ROW()-ROW( $F$154)</f>
+        <v>12,4</v>
+      </c>
+      <c r="S158" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>13,4</v>
+      </c>
+      <c r="T158" s="65" t="str">
+        <f t="shared" si="15"/>
+        <v>14,4</v>
+      </c>
+      <c r="U158" s="29" t="str">
+        <f t="shared" si="15"/>
+        <v>15,4</v>
+      </c>
+    </row>
+    <row r="159" spans="3:21">
+      <c r="F159" s="58" t="str">
+        <f t="shared" si="16"/>
+        <v>0,5</v>
+      </c>
+      <c r="G159" s="59" t="str">
+        <f t="shared" si="15"/>
+        <v>1,5</v>
+      </c>
+      <c r="H159" s="64" t="str">
+        <f t="shared" si="15"/>
+        <v>2,5</v>
+      </c>
+      <c r="I159" s="59" t="str">
+        <f t="shared" si="15"/>
+        <v>3,5</v>
+      </c>
+      <c r="J159" s="60" t="str">
+        <f t="shared" si="15"/>
+        <v>4,5</v>
+      </c>
+      <c r="K159" s="59" t="str">
+        <f t="shared" si="15"/>
+        <v>5,5</v>
+      </c>
+      <c r="L159" s="64" t="str">
+        <f t="shared" si="15"/>
+        <v>6,5</v>
+      </c>
+      <c r="M159" s="61" t="str">
+        <f t="shared" si="15"/>
+        <v>7,5</v>
+      </c>
+      <c r="N159" s="58" t="str">
+        <f t="shared" si="15"/>
+        <v>8,5</v>
+      </c>
+      <c r="O159" s="59" t="str">
+        <f t="shared" si="15"/>
+        <v>9,5</v>
+      </c>
+      <c r="P159" s="64" t="str">
+        <f t="shared" si="15"/>
+        <v>10,5</v>
+      </c>
+      <c r="Q159" s="59" t="str">
+        <f t="shared" si="15"/>
+        <v>11,5</v>
+      </c>
+      <c r="R159" s="60" t="str">
+        <f t="shared" si="15"/>
+        <v>12,5</v>
+      </c>
+      <c r="S159" s="59" t="str">
+        <f t="shared" si="15"/>
+        <v>13,5</v>
+      </c>
+      <c r="T159" s="64" t="str">
+        <f t="shared" si="15"/>
+        <v>14,5</v>
+      </c>
+      <c r="U159" s="61" t="str">
+        <f t="shared" si="15"/>
+        <v>15,5</v>
+      </c>
+    </row>
+    <row r="160" spans="3:21">
+      <c r="F160" s="28" t="str">
+        <f t="shared" si="16"/>
+        <v>0,6</v>
+      </c>
+      <c r="G160" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>1,6</v>
+      </c>
+      <c r="H160" s="65" t="str">
+        <f t="shared" si="15"/>
+        <v>2,6</v>
+      </c>
+      <c r="I160" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>3,6</v>
+      </c>
+      <c r="J160" s="32" t="str">
+        <f t="shared" si="15"/>
+        <v>4,6</v>
+      </c>
+      <c r="K160" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>5,6</v>
+      </c>
+      <c r="L160" s="65" t="str">
+        <f t="shared" si="15"/>
+        <v>6,6</v>
+      </c>
+      <c r="M160" s="29" t="str">
+        <f t="shared" si="15"/>
+        <v>7,6</v>
+      </c>
+      <c r="N160" s="28" t="str">
+        <f t="shared" si="15"/>
+        <v>8,6</v>
+      </c>
+      <c r="O160" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>9,6</v>
+      </c>
+      <c r="P160" s="65" t="str">
+        <f t="shared" si="15"/>
+        <v>10,6</v>
+      </c>
+      <c r="Q160" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>11,6</v>
+      </c>
+      <c r="R160" s="32" t="str">
+        <f t="shared" si="15"/>
+        <v>12,6</v>
+      </c>
+      <c r="S160" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>13,6</v>
+      </c>
+      <c r="T160" s="65" t="str">
+        <f t="shared" si="15"/>
+        <v>14,6</v>
+      </c>
+      <c r="U160" s="29" t="str">
+        <f t="shared" si="15"/>
+        <v>15,6</v>
+      </c>
+    </row>
+    <row r="161" spans="6:21" ht="16" thickBot="1">
+      <c r="F161" s="25" t="str">
+        <f t="shared" si="16"/>
         <v>0,7</v>
       </c>
-      <c r="G90" s="30" t="str">
-        <f t="shared" si="12"/>
+      <c r="G161" s="30" t="str">
+        <f t="shared" si="15"/>
         <v>1,7</v>
       </c>
-      <c r="H90" s="67" t="str">
-        <f t="shared" si="12"/>
+      <c r="H161" s="67" t="str">
+        <f t="shared" si="15"/>
         <v>2,7</v>
       </c>
-      <c r="I90" s="30" t="str">
-        <f t="shared" si="12"/>
+      <c r="I161" s="30" t="str">
+        <f t="shared" si="15"/>
         <v>3,7</v>
       </c>
-      <c r="J90" s="33" t="str">
-        <f t="shared" si="12"/>
+      <c r="J161" s="33" t="str">
+        <f t="shared" si="15"/>
         <v>4,7</v>
       </c>
-      <c r="K90" s="30" t="str">
-        <f t="shared" si="12"/>
+      <c r="K161" s="30" t="str">
+        <f t="shared" si="15"/>
         <v>5,7</v>
       </c>
-      <c r="L90" s="67" t="str">
-        <f t="shared" si="12"/>
+      <c r="L161" s="67" t="str">
+        <f t="shared" si="15"/>
         <v>6,7</v>
       </c>
-      <c r="M90" s="26" t="str">
-        <f t="shared" si="12"/>
+      <c r="M161" s="26" t="str">
+        <f t="shared" si="15"/>
         <v>7,7</v>
+      </c>
+      <c r="N161" s="25" t="str">
+        <f t="shared" si="15"/>
+        <v>8,7</v>
+      </c>
+      <c r="O161" s="30" t="str">
+        <f t="shared" si="15"/>
+        <v>9,7</v>
+      </c>
+      <c r="P161" s="67" t="str">
+        <f t="shared" si="15"/>
+        <v>10,7</v>
+      </c>
+      <c r="Q161" s="30" t="str">
+        <f t="shared" si="15"/>
+        <v>11,7</v>
+      </c>
+      <c r="R161" s="33" t="str">
+        <f t="shared" si="15"/>
+        <v>12,7</v>
+      </c>
+      <c r="S161" s="30" t="str">
+        <f t="shared" si="15"/>
+        <v>13,7</v>
+      </c>
+      <c r="T161" s="67" t="str">
+        <f t="shared" si="15"/>
+        <v>14,7</v>
+      </c>
+      <c r="U161" s="26" t="str">
+        <f t="shared" si="15"/>
+        <v>15,7</v>
+      </c>
+    </row>
+    <row r="162" spans="6:21" ht="17" thickTop="1" thickBot="1">
+      <c r="F162" s="23" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$154) &amp; "," &amp;ROW()-ROW( $F$154)</f>
+        <v>0,8</v>
+      </c>
+      <c r="G162" s="27" t="str">
+        <f t="shared" si="15"/>
+        <v>1,8</v>
+      </c>
+      <c r="H162" s="63" t="str">
+        <f t="shared" si="15"/>
+        <v>2,8</v>
+      </c>
+      <c r="I162" s="27" t="str">
+        <f t="shared" si="15"/>
+        <v>3,8</v>
+      </c>
+      <c r="J162" s="31" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$154) &amp; "," &amp;ROW()-ROW( $F$154)</f>
+        <v>4,8</v>
+      </c>
+      <c r="K162" s="27" t="str">
+        <f t="shared" si="15"/>
+        <v>5,8</v>
+      </c>
+      <c r="L162" s="63" t="str">
+        <f t="shared" si="15"/>
+        <v>6,8</v>
+      </c>
+      <c r="M162" s="24" t="str">
+        <f t="shared" si="15"/>
+        <v>7,8</v>
+      </c>
+      <c r="N162" s="72" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$154) &amp; "," &amp;ROW()-ROW( $F$154)</f>
+        <v>8,8</v>
+      </c>
+      <c r="O162" s="72" t="str">
+        <f t="shared" si="15"/>
+        <v>9,8</v>
+      </c>
+      <c r="P162" s="63" t="str">
+        <f t="shared" si="15"/>
+        <v>10,8</v>
+      </c>
+      <c r="Q162" s="27" t="str">
+        <f t="shared" si="15"/>
+        <v>11,8</v>
+      </c>
+      <c r="R162" s="31" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$154) &amp; "," &amp;ROW()-ROW( $F$154)</f>
+        <v>12,8</v>
+      </c>
+      <c r="S162" s="27" t="str">
+        <f t="shared" si="15"/>
+        <v>13,8</v>
+      </c>
+      <c r="T162" s="63" t="str">
+        <f t="shared" si="15"/>
+        <v>14,8</v>
+      </c>
+      <c r="U162" s="24" t="str">
+        <f t="shared" si="15"/>
+        <v>15,8</v>
+      </c>
+    </row>
+    <row r="163" spans="6:21" ht="17" thickTop="1" thickBot="1">
+      <c r="F163" s="58" t="str">
+        <f t="shared" si="16"/>
+        <v>0,9</v>
+      </c>
+      <c r="G163" s="59" t="str">
+        <f t="shared" si="15"/>
+        <v>1,9</v>
+      </c>
+      <c r="H163" s="64" t="str">
+        <f t="shared" si="15"/>
+        <v>2,9</v>
+      </c>
+      <c r="I163" s="59" t="str">
+        <f t="shared" si="15"/>
+        <v>3,9</v>
+      </c>
+      <c r="J163" s="60" t="str">
+        <f t="shared" si="15"/>
+        <v>4,9</v>
+      </c>
+      <c r="K163" s="59" t="str">
+        <f t="shared" si="15"/>
+        <v>5,9</v>
+      </c>
+      <c r="L163" s="64" t="str">
+        <f t="shared" si="15"/>
+        <v>6,9</v>
+      </c>
+      <c r="M163" s="61" t="str">
+        <f t="shared" si="15"/>
+        <v>7,9</v>
+      </c>
+      <c r="N163" s="72" t="str">
+        <f t="shared" si="15"/>
+        <v>8,9</v>
+      </c>
+      <c r="O163" s="72" t="str">
+        <f t="shared" si="15"/>
+        <v>9,9</v>
+      </c>
+      <c r="P163" s="64" t="str">
+        <f t="shared" si="15"/>
+        <v>10,9</v>
+      </c>
+      <c r="Q163" s="59" t="str">
+        <f t="shared" si="15"/>
+        <v>11,9</v>
+      </c>
+      <c r="R163" s="60" t="str">
+        <f t="shared" si="15"/>
+        <v>12,9</v>
+      </c>
+      <c r="S163" s="59" t="str">
+        <f t="shared" si="15"/>
+        <v>13,9</v>
+      </c>
+      <c r="T163" s="64" t="str">
+        <f t="shared" si="15"/>
+        <v>14,9</v>
+      </c>
+      <c r="U163" s="61" t="str">
+        <f t="shared" si="15"/>
+        <v>15,9</v>
+      </c>
+    </row>
+    <row r="164" spans="6:21" ht="16" thickTop="1">
+      <c r="F164" s="62" t="str">
+        <f t="shared" si="16"/>
+        <v>0,10</v>
+      </c>
+      <c r="G164" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>1,10</v>
+      </c>
+      <c r="H164" s="65" t="str">
+        <f t="shared" si="15"/>
+        <v>2,10</v>
+      </c>
+      <c r="I164" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>3,10</v>
+      </c>
+      <c r="J164" s="32" t="str">
+        <f t="shared" si="15"/>
+        <v>4,10</v>
+      </c>
+      <c r="K164" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>5,10</v>
+      </c>
+      <c r="L164" s="65" t="str">
+        <f t="shared" si="15"/>
+        <v>6,10</v>
+      </c>
+      <c r="M164" s="29" t="str">
+        <f t="shared" si="15"/>
+        <v>7,10</v>
+      </c>
+      <c r="N164" s="62" t="str">
+        <f t="shared" si="15"/>
+        <v>8,10</v>
+      </c>
+      <c r="O164" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>9,10</v>
+      </c>
+      <c r="P164" s="65" t="str">
+        <f t="shared" si="15"/>
+        <v>10,10</v>
+      </c>
+      <c r="Q164" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>11,10</v>
+      </c>
+      <c r="R164" s="32" t="str">
+        <f t="shared" si="15"/>
+        <v>12,10</v>
+      </c>
+      <c r="S164" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>13,10</v>
+      </c>
+      <c r="T164" s="65" t="str">
+        <f t="shared" si="15"/>
+        <v>14,10</v>
+      </c>
+      <c r="U164" s="29" t="str">
+        <f t="shared" si="15"/>
+        <v>15,10</v>
+      </c>
+    </row>
+    <row r="165" spans="6:21">
+      <c r="F165" s="34" t="str">
+        <f t="shared" si="16"/>
+        <v>0,11</v>
+      </c>
+      <c r="G165" s="35" t="str">
+        <f t="shared" si="15"/>
+        <v>1,11</v>
+      </c>
+      <c r="H165" s="66" t="str">
+        <f t="shared" si="15"/>
+        <v>2,11</v>
+      </c>
+      <c r="I165" s="35" t="str">
+        <f t="shared" si="15"/>
+        <v>3,11</v>
+      </c>
+      <c r="J165" s="36" t="str">
+        <f t="shared" si="15"/>
+        <v>4,11</v>
+      </c>
+      <c r="K165" s="35" t="str">
+        <f t="shared" si="15"/>
+        <v>5,11</v>
+      </c>
+      <c r="L165" s="66" t="str">
+        <f t="shared" si="15"/>
+        <v>6,11</v>
+      </c>
+      <c r="M165" s="37" t="str">
+        <f t="shared" si="15"/>
+        <v>7,11</v>
+      </c>
+      <c r="N165" s="34" t="str">
+        <f t="shared" si="15"/>
+        <v>8,11</v>
+      </c>
+      <c r="O165" s="35" t="str">
+        <f t="shared" si="15"/>
+        <v>9,11</v>
+      </c>
+      <c r="P165" s="66" t="str">
+        <f t="shared" si="15"/>
+        <v>10,11</v>
+      </c>
+      <c r="Q165" s="35" t="str">
+        <f t="shared" si="15"/>
+        <v>11,11</v>
+      </c>
+      <c r="R165" s="36" t="str">
+        <f t="shared" si="15"/>
+        <v>12,11</v>
+      </c>
+      <c r="S165" s="35" t="str">
+        <f t="shared" si="15"/>
+        <v>13,11</v>
+      </c>
+      <c r="T165" s="66" t="str">
+        <f t="shared" si="15"/>
+        <v>14,11</v>
+      </c>
+      <c r="U165" s="37" t="str">
+        <f t="shared" si="15"/>
+        <v>15,11</v>
+      </c>
+    </row>
+    <row r="166" spans="6:21">
+      <c r="F166" s="28" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$154) &amp; "," &amp;ROW()-ROW( $F$154)</f>
+        <v>0,12</v>
+      </c>
+      <c r="G166" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>1,12</v>
+      </c>
+      <c r="H166" s="65" t="str">
+        <f t="shared" si="15"/>
+        <v>2,12</v>
+      </c>
+      <c r="I166" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>3,12</v>
+      </c>
+      <c r="J166" s="70" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$154) &amp; "," &amp;ROW()-ROW( $F$154)</f>
+        <v>4,12</v>
+      </c>
+      <c r="K166" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>5,12</v>
+      </c>
+      <c r="L166" s="65" t="str">
+        <f t="shared" si="15"/>
+        <v>6,12</v>
+      </c>
+      <c r="M166" s="29" t="str">
+        <f t="shared" si="15"/>
+        <v>7,12</v>
+      </c>
+      <c r="N166" s="28" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$154) &amp; "," &amp;ROW()-ROW( $F$154)</f>
+        <v>8,12</v>
+      </c>
+      <c r="O166" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>9,12</v>
+      </c>
+      <c r="P166" s="65" t="str">
+        <f t="shared" si="15"/>
+        <v>10,12</v>
+      </c>
+      <c r="Q166" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>11,12</v>
+      </c>
+      <c r="R166" s="70" t="str">
+        <f xml:space="preserve"> COLUMN()-COLUMN( $F$154) &amp; "," &amp;ROW()-ROW( $F$154)</f>
+        <v>12,12</v>
+      </c>
+      <c r="S166" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>13,12</v>
+      </c>
+      <c r="T166" s="65" t="str">
+        <f t="shared" si="15"/>
+        <v>14,12</v>
+      </c>
+      <c r="U166" s="29" t="str">
+        <f t="shared" si="15"/>
+        <v>15,12</v>
+      </c>
+    </row>
+    <row r="167" spans="6:21">
+      <c r="F167" s="58" t="str">
+        <f t="shared" si="16"/>
+        <v>0,13</v>
+      </c>
+      <c r="G167" s="59" t="str">
+        <f t="shared" si="15"/>
+        <v>1,13</v>
+      </c>
+      <c r="H167" s="64" t="str">
+        <f t="shared" si="15"/>
+        <v>2,13</v>
+      </c>
+      <c r="I167" s="59" t="str">
+        <f t="shared" si="15"/>
+        <v>3,13</v>
+      </c>
+      <c r="J167" s="60" t="str">
+        <f t="shared" si="15"/>
+        <v>4,13</v>
+      </c>
+      <c r="K167" s="59" t="str">
+        <f t="shared" si="15"/>
+        <v>5,13</v>
+      </c>
+      <c r="L167" s="64" t="str">
+        <f t="shared" si="15"/>
+        <v>6,13</v>
+      </c>
+      <c r="M167" s="61" t="str">
+        <f t="shared" si="15"/>
+        <v>7,13</v>
+      </c>
+      <c r="N167" s="58" t="str">
+        <f t="shared" si="15"/>
+        <v>8,13</v>
+      </c>
+      <c r="O167" s="59" t="str">
+        <f t="shared" si="15"/>
+        <v>9,13</v>
+      </c>
+      <c r="P167" s="64" t="str">
+        <f t="shared" si="15"/>
+        <v>10,13</v>
+      </c>
+      <c r="Q167" s="59" t="str">
+        <f t="shared" si="15"/>
+        <v>11,13</v>
+      </c>
+      <c r="R167" s="60" t="str">
+        <f t="shared" si="15"/>
+        <v>12,13</v>
+      </c>
+      <c r="S167" s="59" t="str">
+        <f t="shared" si="15"/>
+        <v>13,13</v>
+      </c>
+      <c r="T167" s="64" t="str">
+        <f t="shared" si="15"/>
+        <v>14,13</v>
+      </c>
+      <c r="U167" s="61" t="str">
+        <f t="shared" si="15"/>
+        <v>15,13</v>
+      </c>
+    </row>
+    <row r="168" spans="6:21">
+      <c r="F168" s="28" t="str">
+        <f t="shared" si="16"/>
+        <v>0,14</v>
+      </c>
+      <c r="G168" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>1,14</v>
+      </c>
+      <c r="H168" s="65" t="str">
+        <f t="shared" si="15"/>
+        <v>2,14</v>
+      </c>
+      <c r="I168" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>3,14</v>
+      </c>
+      <c r="J168" s="32" t="str">
+        <f t="shared" si="15"/>
+        <v>4,14</v>
+      </c>
+      <c r="K168" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>5,14</v>
+      </c>
+      <c r="L168" s="65" t="str">
+        <f t="shared" si="15"/>
+        <v>6,14</v>
+      </c>
+      <c r="M168" s="29" t="str">
+        <f t="shared" si="15"/>
+        <v>7,14</v>
+      </c>
+      <c r="N168" s="28" t="str">
+        <f t="shared" si="15"/>
+        <v>8,14</v>
+      </c>
+      <c r="O168" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>9,14</v>
+      </c>
+      <c r="P168" s="65" t="str">
+        <f t="shared" si="15"/>
+        <v>10,14</v>
+      </c>
+      <c r="Q168" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>11,14</v>
+      </c>
+      <c r="R168" s="32" t="str">
+        <f t="shared" si="15"/>
+        <v>12,14</v>
+      </c>
+      <c r="S168" s="22" t="str">
+        <f t="shared" si="15"/>
+        <v>13,14</v>
+      </c>
+      <c r="T168" s="65" t="str">
+        <f t="shared" si="15"/>
+        <v>14,14</v>
+      </c>
+      <c r="U168" s="29" t="str">
+        <f t="shared" si="15"/>
+        <v>15,14</v>
+      </c>
+    </row>
+    <row r="169" spans="6:21" ht="16" thickBot="1">
+      <c r="F169" s="25" t="str">
+        <f t="shared" si="16"/>
+        <v>0,15</v>
+      </c>
+      <c r="G169" s="30" t="str">
+        <f t="shared" si="15"/>
+        <v>1,15</v>
+      </c>
+      <c r="H169" s="67" t="str">
+        <f t="shared" si="15"/>
+        <v>2,15</v>
+      </c>
+      <c r="I169" s="30" t="str">
+        <f t="shared" si="15"/>
+        <v>3,15</v>
+      </c>
+      <c r="J169" s="33" t="str">
+        <f t="shared" si="15"/>
+        <v>4,15</v>
+      </c>
+      <c r="K169" s="30" t="str">
+        <f t="shared" si="15"/>
+        <v>5,15</v>
+      </c>
+      <c r="L169" s="67" t="str">
+        <f t="shared" si="15"/>
+        <v>6,15</v>
+      </c>
+      <c r="M169" s="26" t="str">
+        <f t="shared" si="15"/>
+        <v>7,15</v>
+      </c>
+      <c r="N169" s="25" t="str">
+        <f t="shared" si="15"/>
+        <v>8,15</v>
+      </c>
+      <c r="O169" s="30" t="str">
+        <f t="shared" si="15"/>
+        <v>9,15</v>
+      </c>
+      <c r="P169" s="67" t="str">
+        <f t="shared" si="15"/>
+        <v>10,15</v>
+      </c>
+      <c r="Q169" s="30" t="str">
+        <f t="shared" si="15"/>
+        <v>11,15</v>
+      </c>
+      <c r="R169" s="33" t="str">
+        <f t="shared" si="15"/>
+        <v>12,15</v>
+      </c>
+      <c r="S169" s="30" t="str">
+        <f t="shared" si="15"/>
+        <v>13,15</v>
+      </c>
+      <c r="T169" s="67" t="str">
+        <f t="shared" si="15"/>
+        <v>14,15</v>
+      </c>
+      <c r="U169" s="26" t="str">
+        <f t="shared" si="15"/>
+        <v>15,15</v>
       </c>
     </row>
   </sheetData>
@@ -7737,4 +9900,25 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>